<commit_message>
Added t=5 and t=-1 data
</commit_message>
<xml_diff>
--- a/data/iris_stats.xlsx
+++ b/data/iris_stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choyboy/Documents/Python/TERM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choyboy/Documents/Python/TERM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1B7308-9D5B-B34F-BDED-6684B23C78CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F62353-F3EB-F347-A7FE-214BC1D32CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="2140" windowWidth="28040" windowHeight="17440" xr2:uid="{F4ABBBD4-D0CD-3741-A4C2-0732B8BAB08E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="20">
   <si>
     <t>data_split</t>
   </si>
@@ -514,19 +514,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08A4D35-E706-CC45-B598-207DF2A9E827}">
-  <dimension ref="A1:O91"/>
+  <dimension ref="A1:O181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="111" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O92" sqref="O92"/>
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
+      <selection activeCell="N181" sqref="N181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
@@ -4810,6 +4815,4236 @@
         <v>0.95</v>
       </c>
     </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A92" s="3">
+        <v>1</v>
+      </c>
+      <c r="B92" s="3">
+        <v>0</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92" s="3">
+        <v>5</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G92" s="3">
+        <v>1</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J92" s="3">
+        <v>100</v>
+      </c>
+      <c r="K92" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L92" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="M92" s="5">
+        <v>1</v>
+      </c>
+      <c r="N92" s="5">
+        <v>0.88392857142857095</v>
+      </c>
+      <c r="O92" s="5">
+        <v>0.88571428571428501</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A93" s="3">
+        <v>1</v>
+      </c>
+      <c r="B93" s="3">
+        <v>0</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D93" s="3">
+        <v>5</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G93" s="3">
+        <v>2</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I93" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J93" s="3">
+        <v>100</v>
+      </c>
+      <c r="K93" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L93" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M93" s="5">
+        <v>1</v>
+      </c>
+      <c r="N93" s="5">
+        <v>0.95357142857142796</v>
+      </c>
+      <c r="O93" s="5">
+        <v>0.93571428571428505</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A94" s="3">
+        <v>1</v>
+      </c>
+      <c r="B94" s="3">
+        <v>0</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D94" s="3">
+        <v>5</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G94" s="3">
+        <v>3</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J94" s="3">
+        <v>100</v>
+      </c>
+      <c r="K94" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L94" s="5">
+        <v>1</v>
+      </c>
+      <c r="M94" s="5">
+        <v>1</v>
+      </c>
+      <c r="N94" s="5">
+        <v>0.97321428571428503</v>
+      </c>
+      <c r="O94" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A95" s="3">
+        <v>1</v>
+      </c>
+      <c r="B95" s="3">
+        <v>1</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95" s="3">
+        <v>5</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G95" s="3">
+        <v>1</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I95" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J95" s="3">
+        <v>100</v>
+      </c>
+      <c r="K95" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L95" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="M95" s="5">
+        <v>1</v>
+      </c>
+      <c r="N95" s="5">
+        <v>0.89285714285714202</v>
+      </c>
+      <c r="O95" s="5">
+        <v>0.94285714285714195</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A96" s="3">
+        <v>1</v>
+      </c>
+      <c r="B96" s="3">
+        <v>1</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D96" s="3">
+        <v>5</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G96" s="3">
+        <v>2</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I96" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J96" s="3">
+        <v>100</v>
+      </c>
+      <c r="K96" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L96" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M96" s="5">
+        <v>1</v>
+      </c>
+      <c r="N96" s="5">
+        <v>0.95535714285714202</v>
+      </c>
+      <c r="O96" s="5">
+        <v>0.99285714285714199</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A97" s="3">
+        <v>1</v>
+      </c>
+      <c r="B97" s="3">
+        <v>1</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D97" s="3">
+        <v>5</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G97" s="3">
+        <v>3</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J97" s="3">
+        <v>100</v>
+      </c>
+      <c r="K97" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L97" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M97" s="5">
+        <v>1</v>
+      </c>
+      <c r="N97" s="5">
+        <v>0.97142857142857097</v>
+      </c>
+      <c r="O97" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A98" s="3">
+        <v>1</v>
+      </c>
+      <c r="B98" s="3">
+        <v>2</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D98" s="3">
+        <v>5</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G98" s="3">
+        <v>1</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J98" s="3">
+        <v>100</v>
+      </c>
+      <c r="K98" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L98" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="M98" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="N98" s="5">
+        <v>0.88035714285714195</v>
+      </c>
+      <c r="O98" s="5">
+        <v>0.84285714285714197</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A99" s="3">
+        <v>1</v>
+      </c>
+      <c r="B99" s="3">
+        <v>2</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D99" s="3">
+        <v>5</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G99" s="3">
+        <v>2</v>
+      </c>
+      <c r="H99" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I99" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J99" s="3">
+        <v>100</v>
+      </c>
+      <c r="K99" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L99" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M99" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="N99" s="5">
+        <v>0.9375</v>
+      </c>
+      <c r="O99" s="5">
+        <v>0.89285714285714202</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A100" s="3">
+        <v>1</v>
+      </c>
+      <c r="B100" s="3">
+        <v>2</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D100" s="3">
+        <v>5</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G100" s="3">
+        <v>3</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I100" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J100" s="3">
+        <v>100</v>
+      </c>
+      <c r="K100" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L100" s="5">
+        <v>1</v>
+      </c>
+      <c r="M100" s="5">
+        <v>1</v>
+      </c>
+      <c r="N100" s="5">
+        <v>0.97857142857142798</v>
+      </c>
+      <c r="O100" s="5">
+        <v>0.92142857142857104</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A101" s="3">
+        <v>2</v>
+      </c>
+      <c r="B101" s="3">
+        <v>0</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D101" s="3">
+        <v>5</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G101" s="3">
+        <v>1</v>
+      </c>
+      <c r="H101" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I101" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J101" s="3">
+        <v>100</v>
+      </c>
+      <c r="K101" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L101" s="5">
+        <v>0.94642857142857095</v>
+      </c>
+      <c r="M101" s="5">
+        <v>1</v>
+      </c>
+      <c r="N101" s="5">
+        <v>0.88214285714285701</v>
+      </c>
+      <c r="O101" s="5">
+        <v>0.90714285714285703</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A102" s="3">
+        <v>2</v>
+      </c>
+      <c r="B102" s="3">
+        <v>0</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D102" s="3">
+        <v>5</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G102" s="3">
+        <v>2</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J102" s="3">
+        <v>100</v>
+      </c>
+      <c r="K102" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L102" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M102" s="5">
+        <v>1</v>
+      </c>
+      <c r="N102" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="O102" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A103" s="3">
+        <v>2</v>
+      </c>
+      <c r="B103" s="3">
+        <v>0</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D103" s="3">
+        <v>5</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G103" s="3">
+        <v>3</v>
+      </c>
+      <c r="H103" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I103" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J103" s="3">
+        <v>100</v>
+      </c>
+      <c r="K103" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L103" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M103" s="5">
+        <v>1</v>
+      </c>
+      <c r="N103" s="5">
+        <v>0.97857142857142798</v>
+      </c>
+      <c r="O103" s="5">
+        <v>0.97142857142857097</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A104" s="3">
+        <v>2</v>
+      </c>
+      <c r="B104" s="3">
+        <v>1</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D104" s="3">
+        <v>5</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G104" s="3">
+        <v>1</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J104" s="3">
+        <v>100</v>
+      </c>
+      <c r="K104" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L104" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="M104" s="5">
+        <v>1</v>
+      </c>
+      <c r="N104" s="5">
+        <v>0.89464285714285696</v>
+      </c>
+      <c r="O104" s="5">
+        <v>0.878571428571428</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A105" s="3">
+        <v>2</v>
+      </c>
+      <c r="B105" s="3">
+        <v>1</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D105" s="3">
+        <v>5</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G105" s="3">
+        <v>2</v>
+      </c>
+      <c r="H105" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I105" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" s="3">
+        <v>100</v>
+      </c>
+      <c r="K105" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L105" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M105" s="5">
+        <v>1</v>
+      </c>
+      <c r="N105" s="5">
+        <v>0.94642857142857095</v>
+      </c>
+      <c r="O105" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A106" s="3">
+        <v>2</v>
+      </c>
+      <c r="B106" s="3">
+        <v>1</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D106" s="3">
+        <v>5</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G106" s="3">
+        <v>3</v>
+      </c>
+      <c r="H106" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I106" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J106" s="3">
+        <v>100</v>
+      </c>
+      <c r="K106" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L106" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M106" s="5">
+        <v>1</v>
+      </c>
+      <c r="N106" s="5">
+        <v>0.9375</v>
+      </c>
+      <c r="O106" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A107" s="3">
+        <v>2</v>
+      </c>
+      <c r="B107" s="3">
+        <v>2</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D107" s="3">
+        <v>5</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G107" s="3">
+        <v>1</v>
+      </c>
+      <c r="H107" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I107" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J107" s="3">
+        <v>100</v>
+      </c>
+      <c r="K107" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L107" s="5">
+        <v>0.83928571428571397</v>
+      </c>
+      <c r="M107" s="5">
+        <v>0.85714285714285698</v>
+      </c>
+      <c r="N107" s="5">
+        <v>0.78749999999999998</v>
+      </c>
+      <c r="O107" s="5">
+        <v>0.75714285714285701</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A108" s="3">
+        <v>2</v>
+      </c>
+      <c r="B108" s="3">
+        <v>2</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D108" s="3">
+        <v>5</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G108" s="3">
+        <v>2</v>
+      </c>
+      <c r="H108" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J108" s="3">
+        <v>100</v>
+      </c>
+      <c r="K108" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L108" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M108" s="5">
+        <v>1</v>
+      </c>
+      <c r="N108" s="5">
+        <v>0.90892857142857097</v>
+      </c>
+      <c r="O108" s="5">
+        <v>0.90714285714285703</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A109" s="3">
+        <v>2</v>
+      </c>
+      <c r="B109" s="3">
+        <v>2</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D109" s="3">
+        <v>5</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G109" s="3">
+        <v>3</v>
+      </c>
+      <c r="H109" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I109" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J109" s="3">
+        <v>100</v>
+      </c>
+      <c r="K109" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L109" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M109" s="5">
+        <v>1</v>
+      </c>
+      <c r="N109" s="5">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="O109" s="5">
+        <v>0.97142857142857097</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A110" s="3">
+        <v>3</v>
+      </c>
+      <c r="B110" s="3">
+        <v>0</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D110" s="3">
+        <v>5</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G110" s="3">
+        <v>1</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J110" s="3">
+        <v>100</v>
+      </c>
+      <c r="K110" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L110" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M110" s="5">
+        <v>1</v>
+      </c>
+      <c r="N110" s="5">
+        <v>0.88392857142857095</v>
+      </c>
+      <c r="O110" s="5">
+        <v>0.88571428571428501</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A111" s="3">
+        <v>3</v>
+      </c>
+      <c r="B111" s="3">
+        <v>0</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D111" s="3">
+        <v>5</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G111" s="3">
+        <v>2</v>
+      </c>
+      <c r="H111" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J111" s="3">
+        <v>100</v>
+      </c>
+      <c r="K111" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L111" s="5">
+        <v>1</v>
+      </c>
+      <c r="M111" s="5">
+        <v>1</v>
+      </c>
+      <c r="N111" s="5">
+        <v>0.97321428571428503</v>
+      </c>
+      <c r="O111" s="5">
+        <v>0.99285714285714199</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A112" s="3">
+        <v>3</v>
+      </c>
+      <c r="B112" s="3">
+        <v>0</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D112" s="3">
+        <v>5</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G112" s="3">
+        <v>3</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J112" s="3">
+        <v>100</v>
+      </c>
+      <c r="K112" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L112" s="5">
+        <v>1</v>
+      </c>
+      <c r="M112" s="5">
+        <v>1</v>
+      </c>
+      <c r="N112" s="5">
+        <v>0.98392857142857104</v>
+      </c>
+      <c r="O112" s="5">
+        <v>0.99285714285714199</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A113" s="3">
+        <v>3</v>
+      </c>
+      <c r="B113" s="3">
+        <v>1</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D113" s="3">
+        <v>5</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G113" s="3">
+        <v>1</v>
+      </c>
+      <c r="H113" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I113" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J113" s="3">
+        <v>100</v>
+      </c>
+      <c r="K113" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L113" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M113" s="5">
+        <v>1</v>
+      </c>
+      <c r="N113" s="5">
+        <v>0.92678571428571399</v>
+      </c>
+      <c r="O113" s="5">
+        <v>0.97857142857142798</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A114" s="3">
+        <v>3</v>
+      </c>
+      <c r="B114" s="3">
+        <v>1</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D114" s="3">
+        <v>5</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G114" s="3">
+        <v>2</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J114" s="3">
+        <v>100</v>
+      </c>
+      <c r="K114" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L114" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M114" s="5">
+        <v>1</v>
+      </c>
+      <c r="N114" s="5">
+        <v>0.94464285714285701</v>
+      </c>
+      <c r="O114" s="5">
+        <v>0.97142857142857097</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A115" s="3">
+        <v>3</v>
+      </c>
+      <c r="B115" s="3">
+        <v>1</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D115" s="3">
+        <v>5</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G115" s="3">
+        <v>3</v>
+      </c>
+      <c r="H115" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J115" s="3">
+        <v>100</v>
+      </c>
+      <c r="K115" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L115" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M115" s="5">
+        <v>1</v>
+      </c>
+      <c r="N115" s="5">
+        <v>0.96964285714285703</v>
+      </c>
+      <c r="O115" s="5">
+        <v>0.98571428571428499</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A116" s="3">
+        <v>3</v>
+      </c>
+      <c r="B116" s="3">
+        <v>2</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D116" s="3">
+        <v>5</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G116" s="3">
+        <v>1</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J116" s="3">
+        <v>100</v>
+      </c>
+      <c r="K116" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L116" s="5">
+        <v>0.89285714285714202</v>
+      </c>
+      <c r="M116" s="5">
+        <v>0.85714285714285698</v>
+      </c>
+      <c r="N116" s="5">
+        <v>0.83392857142857102</v>
+      </c>
+      <c r="O116" s="5">
+        <v>0.81428571428571395</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A117" s="3">
+        <v>3</v>
+      </c>
+      <c r="B117" s="3">
+        <v>2</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D117" s="3">
+        <v>5</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G117" s="3">
+        <v>2</v>
+      </c>
+      <c r="H117" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J117" s="3">
+        <v>100</v>
+      </c>
+      <c r="K117" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L117" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="M117" s="5">
+        <v>1</v>
+      </c>
+      <c r="N117" s="5">
+        <v>0.93214285714285705</v>
+      </c>
+      <c r="O117" s="5">
+        <v>0.90714285714285703</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A118" s="3">
+        <v>3</v>
+      </c>
+      <c r="B118" s="3">
+        <v>2</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D118" s="3">
+        <v>5</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G118" s="3">
+        <v>3</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J118" s="3">
+        <v>100</v>
+      </c>
+      <c r="K118" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L118" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M118" s="5">
+        <v>1</v>
+      </c>
+      <c r="N118" s="5">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="O118" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A119" s="3">
+        <v>4</v>
+      </c>
+      <c r="B119" s="3">
+        <v>0</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D119" s="3">
+        <v>5</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G119" s="3">
+        <v>1</v>
+      </c>
+      <c r="H119" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I119" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J119" s="3">
+        <v>100</v>
+      </c>
+      <c r="K119" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L119" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="M119" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="N119" s="5">
+        <v>0.90357142857142803</v>
+      </c>
+      <c r="O119" s="5">
+        <v>0.89285714285714202</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A120" s="3">
+        <v>4</v>
+      </c>
+      <c r="B120" s="3">
+        <v>0</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D120" s="3">
+        <v>5</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G120" s="3">
+        <v>2</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J120" s="3">
+        <v>100</v>
+      </c>
+      <c r="K120" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L120" s="5">
+        <v>1</v>
+      </c>
+      <c r="M120" s="5">
+        <v>1</v>
+      </c>
+      <c r="N120" s="5">
+        <v>0.95892857142857102</v>
+      </c>
+      <c r="O120" s="5">
+        <v>0.95714285714285696</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A121" s="3">
+        <v>4</v>
+      </c>
+      <c r="B121" s="3">
+        <v>0</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D121" s="3">
+        <v>5</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G121" s="3">
+        <v>3</v>
+      </c>
+      <c r="H121" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J121" s="3">
+        <v>100</v>
+      </c>
+      <c r="K121" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L121" s="5">
+        <v>1</v>
+      </c>
+      <c r="M121" s="5">
+        <v>1</v>
+      </c>
+      <c r="N121" s="5">
+        <v>0.98392857142857104</v>
+      </c>
+      <c r="O121" s="5">
+        <v>0.98571428571428499</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A122" s="3">
+        <v>4</v>
+      </c>
+      <c r="B122" s="3">
+        <v>1</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D122" s="3">
+        <v>5</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G122" s="3">
+        <v>1</v>
+      </c>
+      <c r="H122" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J122" s="3">
+        <v>100</v>
+      </c>
+      <c r="K122" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L122" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M122" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="N122" s="5">
+        <v>0.89107142857142796</v>
+      </c>
+      <c r="O122" s="5">
+        <v>0.84285714285714197</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A123" s="3">
+        <v>4</v>
+      </c>
+      <c r="B123" s="3">
+        <v>1</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D123" s="3">
+        <v>5</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G123" s="3">
+        <v>2</v>
+      </c>
+      <c r="H123" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J123" s="3">
+        <v>100</v>
+      </c>
+      <c r="K123" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L123" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M123" s="5">
+        <v>1</v>
+      </c>
+      <c r="N123" s="5">
+        <v>0.94464285714285601</v>
+      </c>
+      <c r="O123" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A124" s="3">
+        <v>4</v>
+      </c>
+      <c r="B124" s="3">
+        <v>1</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D124" s="3">
+        <v>5</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G124" s="3">
+        <v>3</v>
+      </c>
+      <c r="H124" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J124" s="3">
+        <v>100</v>
+      </c>
+      <c r="K124" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L124" s="5">
+        <v>1</v>
+      </c>
+      <c r="M124" s="5">
+        <v>1</v>
+      </c>
+      <c r="N124" s="5">
+        <v>0.98928571428571399</v>
+      </c>
+      <c r="O124" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A125" s="3">
+        <v>4</v>
+      </c>
+      <c r="B125" s="3">
+        <v>2</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D125" s="3">
+        <v>5</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G125" s="3">
+        <v>1</v>
+      </c>
+      <c r="H125" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I125" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J125" s="3">
+        <v>100</v>
+      </c>
+      <c r="K125" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L125" s="5">
+        <v>0.91071428571428503</v>
+      </c>
+      <c r="M125" s="5">
+        <v>1</v>
+      </c>
+      <c r="N125" s="5">
+        <v>0.81964285714285701</v>
+      </c>
+      <c r="O125" s="5">
+        <v>0.81428571428571395</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A126" s="3">
+        <v>4</v>
+      </c>
+      <c r="B126" s="3">
+        <v>2</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D126" s="3">
+        <v>5</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G126" s="3">
+        <v>2</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I126" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J126" s="3">
+        <v>100</v>
+      </c>
+      <c r="K126" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L126" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M126" s="5">
+        <v>1</v>
+      </c>
+      <c r="N126" s="5">
+        <v>0.93571428571428505</v>
+      </c>
+      <c r="O126" s="5">
+        <v>0.98571428571428499</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A127" s="3">
+        <v>4</v>
+      </c>
+      <c r="B127" s="3">
+        <v>2</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D127" s="3">
+        <v>5</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F127" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G127" s="3">
+        <v>3</v>
+      </c>
+      <c r="H127" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J127" s="3">
+        <v>100</v>
+      </c>
+      <c r="K127" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L127" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M127" s="5">
+        <v>1</v>
+      </c>
+      <c r="N127" s="5">
+        <v>0.96607142857142803</v>
+      </c>
+      <c r="O127" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A128" s="3">
+        <v>5</v>
+      </c>
+      <c r="B128" s="3">
+        <v>0</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D128" s="3">
+        <v>5</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G128" s="3">
+        <v>1</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J128" s="3">
+        <v>100</v>
+      </c>
+      <c r="K128" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L128" s="5">
+        <v>0.94642857142857095</v>
+      </c>
+      <c r="M128" s="5">
+        <v>1</v>
+      </c>
+      <c r="N128" s="5">
+        <v>0.90357142857142803</v>
+      </c>
+      <c r="O128" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A129" s="3">
+        <v>5</v>
+      </c>
+      <c r="B129" s="3">
+        <v>0</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D129" s="3">
+        <v>5</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G129" s="3">
+        <v>2</v>
+      </c>
+      <c r="H129" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I129" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J129" s="3">
+        <v>100</v>
+      </c>
+      <c r="K129" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L129" s="5">
+        <v>1</v>
+      </c>
+      <c r="M129" s="5">
+        <v>1</v>
+      </c>
+      <c r="N129" s="5">
+        <v>0.96785714285714197</v>
+      </c>
+      <c r="O129" s="5">
+        <v>0.95714285714285696</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A130" s="3">
+        <v>5</v>
+      </c>
+      <c r="B130" s="3">
+        <v>0</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D130" s="3">
+        <v>5</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G130" s="3">
+        <v>3</v>
+      </c>
+      <c r="H130" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I130" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J130" s="3">
+        <v>100</v>
+      </c>
+      <c r="K130" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L130" s="5">
+        <v>1</v>
+      </c>
+      <c r="M130" s="5">
+        <v>1</v>
+      </c>
+      <c r="N130" s="5">
+        <v>1</v>
+      </c>
+      <c r="O130" s="5">
+        <v>0.99285714285714199</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A131" s="3">
+        <v>5</v>
+      </c>
+      <c r="B131" s="3">
+        <v>1</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D131" s="3">
+        <v>5</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F131" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G131" s="3">
+        <v>1</v>
+      </c>
+      <c r="H131" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I131" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J131" s="3">
+        <v>100</v>
+      </c>
+      <c r="K131" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L131" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="M131" s="5">
+        <v>1</v>
+      </c>
+      <c r="N131" s="5">
+        <v>0.92499999999999905</v>
+      </c>
+      <c r="O131" s="5">
+        <v>0.89285714285714202</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A132" s="3">
+        <v>5</v>
+      </c>
+      <c r="B132" s="3">
+        <v>1</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D132" s="3">
+        <v>5</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G132" s="3">
+        <v>2</v>
+      </c>
+      <c r="H132" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I132" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J132" s="3">
+        <v>100</v>
+      </c>
+      <c r="K132" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L132" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M132" s="5">
+        <v>1</v>
+      </c>
+      <c r="N132" s="5">
+        <v>0.97678571428571404</v>
+      </c>
+      <c r="O132" s="5">
+        <v>0.97142857142857097</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A133" s="3">
+        <v>5</v>
+      </c>
+      <c r="B133" s="3">
+        <v>1</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D133" s="3">
+        <v>5</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G133" s="3">
+        <v>3</v>
+      </c>
+      <c r="H133" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I133" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J133" s="3">
+        <v>100</v>
+      </c>
+      <c r="K133" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L133" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M133" s="5">
+        <v>1</v>
+      </c>
+      <c r="N133" s="5">
+        <v>0.97678571428571404</v>
+      </c>
+      <c r="O133" s="5">
+        <v>0.97857142857142798</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A134" s="3">
+        <v>5</v>
+      </c>
+      <c r="B134" s="3">
+        <v>2</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D134" s="3">
+        <v>5</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G134" s="3">
+        <v>1</v>
+      </c>
+      <c r="H134" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J134" s="3">
+        <v>100</v>
+      </c>
+      <c r="K134" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L134" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="M134" s="5">
+        <v>0.97857142857142798</v>
+      </c>
+      <c r="N134" s="5">
+        <v>0.87678571428571395</v>
+      </c>
+      <c r="O134" s="5">
+        <v>0.80714285714285705</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A135" s="3">
+        <v>5</v>
+      </c>
+      <c r="B135" s="3">
+        <v>2</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D135" s="3">
+        <v>5</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G135" s="3">
+        <v>2</v>
+      </c>
+      <c r="H135" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I135" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J135" s="3">
+        <v>100</v>
+      </c>
+      <c r="K135" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L135" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="M135" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="N135" s="5">
+        <v>0.91785714285714204</v>
+      </c>
+      <c r="O135" s="5">
+        <v>0.85714285714285698</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A136" s="3">
+        <v>5</v>
+      </c>
+      <c r="B136" s="3">
+        <v>2</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D136" s="3">
+        <v>5</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G136" s="3">
+        <v>3</v>
+      </c>
+      <c r="H136" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J136" s="3">
+        <v>100</v>
+      </c>
+      <c r="K136" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L136" s="5">
+        <v>1</v>
+      </c>
+      <c r="M136" s="5">
+        <v>1</v>
+      </c>
+      <c r="N136" s="5">
+        <v>0.99285714285714199</v>
+      </c>
+      <c r="O136" s="5">
+        <v>0.95714285714285696</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A137" s="3">
+        <v>1</v>
+      </c>
+      <c r="B137" s="3">
+        <v>0</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D137" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G137" s="3">
+        <v>1</v>
+      </c>
+      <c r="H137" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I137" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J137" s="3">
+        <v>100</v>
+      </c>
+      <c r="K137" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L137" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="M137" s="5">
+        <v>1</v>
+      </c>
+      <c r="N137" s="5">
+        <v>0.88392857142857095</v>
+      </c>
+      <c r="O137" s="5">
+        <v>0.878571428571428</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A138" s="3">
+        <v>1</v>
+      </c>
+      <c r="B138" s="3">
+        <v>0</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D138" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G138" s="3">
+        <v>2</v>
+      </c>
+      <c r="H138" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J138" s="3">
+        <v>100</v>
+      </c>
+      <c r="K138" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L138" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M138" s="5">
+        <v>1</v>
+      </c>
+      <c r="N138" s="5">
+        <v>0.96071428571428497</v>
+      </c>
+      <c r="O138" s="5">
+        <v>0.92142857142857104</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A139" s="3">
+        <v>1</v>
+      </c>
+      <c r="B139" s="3">
+        <v>0</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D139" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E139" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G139" s="3">
+        <v>3</v>
+      </c>
+      <c r="H139" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I139" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J139" s="3">
+        <v>100</v>
+      </c>
+      <c r="K139" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L139" s="5">
+        <v>1</v>
+      </c>
+      <c r="M139" s="5">
+        <v>1</v>
+      </c>
+      <c r="N139" s="5">
+        <v>0.97321428571428503</v>
+      </c>
+      <c r="O139" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A140" s="3">
+        <v>1</v>
+      </c>
+      <c r="B140" s="3">
+        <v>1</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D140" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G140" s="3">
+        <v>1</v>
+      </c>
+      <c r="H140" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I140" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J140" s="3">
+        <v>100</v>
+      </c>
+      <c r="K140" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L140" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="M140" s="5">
+        <v>1</v>
+      </c>
+      <c r="N140" s="5">
+        <v>0.89642857142857102</v>
+      </c>
+      <c r="O140" s="5">
+        <v>0.93571428571428505</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A141" s="3">
+        <v>1</v>
+      </c>
+      <c r="B141" s="3">
+        <v>1</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D141" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F141" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G141" s="3">
+        <v>2</v>
+      </c>
+      <c r="H141" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I141" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J141" s="3">
+        <v>100</v>
+      </c>
+      <c r="K141" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L141" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="M141" s="5">
+        <v>1</v>
+      </c>
+      <c r="N141" s="5">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="O141" s="5">
+        <v>0.97142857142857097</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A142" s="3">
+        <v>1</v>
+      </c>
+      <c r="B142" s="3">
+        <v>1</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D142" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G142" s="3">
+        <v>3</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I142" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J142" s="3">
+        <v>100</v>
+      </c>
+      <c r="K142" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L142" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="M142" s="5">
+        <v>1</v>
+      </c>
+      <c r="N142" s="5">
+        <v>0.941071428571428</v>
+      </c>
+      <c r="O142" s="5">
+        <v>0.98571428571428499</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A143" s="3">
+        <v>1</v>
+      </c>
+      <c r="B143" s="3">
+        <v>2</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D143" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F143" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G143" s="3">
+        <v>1</v>
+      </c>
+      <c r="H143" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I143" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J143" s="3">
+        <v>100</v>
+      </c>
+      <c r="K143" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L143" s="5">
+        <v>0.89285714285714202</v>
+      </c>
+      <c r="M143" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="N143" s="5">
+        <v>0.82857142857142796</v>
+      </c>
+      <c r="O143" s="5">
+        <v>0.85714285714285698</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A144" s="3">
+        <v>1</v>
+      </c>
+      <c r="B144" s="3">
+        <v>2</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D144" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E144" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F144" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G144" s="3">
+        <v>2</v>
+      </c>
+      <c r="H144" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I144" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J144" s="3">
+        <v>100</v>
+      </c>
+      <c r="K144" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L144" s="5">
+        <v>0.94642857142857095</v>
+      </c>
+      <c r="M144" s="5">
+        <v>0.85714285714285698</v>
+      </c>
+      <c r="N144" s="5">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="O144" s="5">
+        <v>0.85714285714285698</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A145" s="3">
+        <v>1</v>
+      </c>
+      <c r="B145" s="3">
+        <v>2</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D145" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G145" s="3">
+        <v>3</v>
+      </c>
+      <c r="H145" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I145" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J145" s="3">
+        <v>100</v>
+      </c>
+      <c r="K145" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L145" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="M145" s="5">
+        <v>1</v>
+      </c>
+      <c r="N145" s="5">
+        <v>0.941071428571428</v>
+      </c>
+      <c r="O145" s="5">
+        <v>0.90714285714285703</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A146" s="3">
+        <v>2</v>
+      </c>
+      <c r="B146" s="3">
+        <v>0</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D146" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F146" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G146" s="3">
+        <v>1</v>
+      </c>
+      <c r="H146" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I146" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J146" s="3">
+        <v>100</v>
+      </c>
+      <c r="K146" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L146" s="5">
+        <v>0.91071428571428503</v>
+      </c>
+      <c r="M146" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="N146" s="5">
+        <v>0.86071428571428499</v>
+      </c>
+      <c r="O146" s="5">
+        <v>0.86428571428571399</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A147" s="3">
+        <v>2</v>
+      </c>
+      <c r="B147" s="3">
+        <v>0</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D147" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F147" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G147" s="3">
+        <v>2</v>
+      </c>
+      <c r="H147" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I147" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J147" s="3">
+        <v>100</v>
+      </c>
+      <c r="K147" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L147" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="M147" s="5">
+        <v>1</v>
+      </c>
+      <c r="N147" s="5">
+        <v>0.941071428571428</v>
+      </c>
+      <c r="O147" s="5">
+        <v>0.97142857142857097</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A148" s="3">
+        <v>2</v>
+      </c>
+      <c r="B148" s="3">
+        <v>0</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D148" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E148" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F148" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G148" s="3">
+        <v>3</v>
+      </c>
+      <c r="H148" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I148" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J148" s="3">
+        <v>100</v>
+      </c>
+      <c r="K148" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L148" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M148" s="5">
+        <v>1</v>
+      </c>
+      <c r="N148" s="5">
+        <v>0.95178571428571401</v>
+      </c>
+      <c r="O148" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A149" s="3">
+        <v>2</v>
+      </c>
+      <c r="B149" s="3">
+        <v>1</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D149" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F149" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G149" s="3">
+        <v>1</v>
+      </c>
+      <c r="H149" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I149" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J149" s="3">
+        <v>100</v>
+      </c>
+      <c r="K149" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L149" s="5">
+        <v>0.91071428571428503</v>
+      </c>
+      <c r="M149" s="5">
+        <v>1</v>
+      </c>
+      <c r="N149" s="5">
+        <v>0.85892857142857104</v>
+      </c>
+      <c r="O149" s="5">
+        <v>0.86428571428571399</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A150" s="3">
+        <v>2</v>
+      </c>
+      <c r="B150" s="3">
+        <v>1</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D150" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G150" s="3">
+        <v>2</v>
+      </c>
+      <c r="H150" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I150" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J150" s="3">
+        <v>100</v>
+      </c>
+      <c r="K150" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L150" s="5">
+        <v>0.94642857142857095</v>
+      </c>
+      <c r="M150" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="N150" s="5">
+        <v>0.90535714285714197</v>
+      </c>
+      <c r="O150" s="5">
+        <v>0.90714285714285703</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A151" s="3">
+        <v>2</v>
+      </c>
+      <c r="B151" s="3">
+        <v>1</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D151" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G151" s="3">
+        <v>3</v>
+      </c>
+      <c r="H151" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I151" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J151" s="3">
+        <v>100</v>
+      </c>
+      <c r="K151" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L151" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="M151" s="5">
+        <v>1</v>
+      </c>
+      <c r="N151" s="5">
+        <v>0.94464285714285701</v>
+      </c>
+      <c r="O151" s="5">
+        <v>0.94285714285714195</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A152" s="3">
+        <v>2</v>
+      </c>
+      <c r="B152" s="3">
+        <v>2</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D152" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G152" s="3">
+        <v>1</v>
+      </c>
+      <c r="H152" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I152" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J152" s="3">
+        <v>100</v>
+      </c>
+      <c r="K152" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L152" s="5">
+        <v>0.89285714285714202</v>
+      </c>
+      <c r="M152" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="N152" s="5">
+        <v>0.82857142857142796</v>
+      </c>
+      <c r="O152" s="5">
+        <v>0.82142857142857095</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A153" s="3">
+        <v>2</v>
+      </c>
+      <c r="B153" s="3">
+        <v>2</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D153" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F153" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G153" s="3">
+        <v>2</v>
+      </c>
+      <c r="H153" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I153" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J153" s="3">
+        <v>100</v>
+      </c>
+      <c r="K153" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L153" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="M153" s="5">
+        <v>1</v>
+      </c>
+      <c r="N153" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="O153" s="5">
+        <v>0.90714285714285703</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A154" s="3">
+        <v>2</v>
+      </c>
+      <c r="B154" s="3">
+        <v>2</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D154" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F154" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G154" s="3">
+        <v>3</v>
+      </c>
+      <c r="H154" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I154" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J154" s="3">
+        <v>100</v>
+      </c>
+      <c r="K154" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L154" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="M154" s="5">
+        <v>1</v>
+      </c>
+      <c r="N154" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="O154" s="5">
+        <v>0.97142857142857097</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A155" s="3">
+        <v>3</v>
+      </c>
+      <c r="B155" s="3">
+        <v>0</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D155" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E155" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G155" s="3">
+        <v>1</v>
+      </c>
+      <c r="H155" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I155" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J155" s="3">
+        <v>100</v>
+      </c>
+      <c r="K155" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L155" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="M155" s="5">
+        <v>1</v>
+      </c>
+      <c r="N155" s="5">
+        <v>0.89821428571428497</v>
+      </c>
+      <c r="O155" s="5">
+        <v>0.90714285714285703</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A156" s="3">
+        <v>3</v>
+      </c>
+      <c r="B156" s="3">
+        <v>0</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D156" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F156" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G156" s="3">
+        <v>2</v>
+      </c>
+      <c r="H156" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I156" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J156" s="3">
+        <v>100</v>
+      </c>
+      <c r="K156" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L156" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M156" s="5">
+        <v>1</v>
+      </c>
+      <c r="N156" s="5">
+        <v>0.96071428571428497</v>
+      </c>
+      <c r="O156" s="5">
+        <v>0.97857142857142798</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A157" s="3">
+        <v>3</v>
+      </c>
+      <c r="B157" s="3">
+        <v>0</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D157" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G157" s="3">
+        <v>3</v>
+      </c>
+      <c r="H157" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I157" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J157" s="3">
+        <v>100</v>
+      </c>
+      <c r="K157" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L157" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M157" s="5">
+        <v>1</v>
+      </c>
+      <c r="N157" s="5">
+        <v>0.97142857142857097</v>
+      </c>
+      <c r="O157" s="5">
+        <v>0.99285714285714199</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A158" s="3">
+        <v>3</v>
+      </c>
+      <c r="B158" s="3">
+        <v>1</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D158" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G158" s="3">
+        <v>1</v>
+      </c>
+      <c r="H158" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I158" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J158" s="3">
+        <v>100</v>
+      </c>
+      <c r="K158" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L158" s="5">
+        <v>0.94642857142857095</v>
+      </c>
+      <c r="M158" s="5">
+        <v>1</v>
+      </c>
+      <c r="N158" s="5">
+        <v>0.88928571428571401</v>
+      </c>
+      <c r="O158" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A159" s="3">
+        <v>3</v>
+      </c>
+      <c r="B159" s="3">
+        <v>1</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D159" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G159" s="3">
+        <v>2</v>
+      </c>
+      <c r="H159" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I159" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J159" s="3">
+        <v>100</v>
+      </c>
+      <c r="K159" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L159" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M159" s="5">
+        <v>1</v>
+      </c>
+      <c r="N159" s="5">
+        <v>0.95714285714285696</v>
+      </c>
+      <c r="O159" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A160" s="3">
+        <v>3</v>
+      </c>
+      <c r="B160" s="3">
+        <v>1</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D160" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G160" s="3">
+        <v>3</v>
+      </c>
+      <c r="H160" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I160" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J160" s="3">
+        <v>100</v>
+      </c>
+      <c r="K160" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L160" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M160" s="5">
+        <v>1</v>
+      </c>
+      <c r="N160" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="O160" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A161" s="3">
+        <v>3</v>
+      </c>
+      <c r="B161" s="3">
+        <v>2</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D161" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F161" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G161" s="3">
+        <v>1</v>
+      </c>
+      <c r="H161" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I161" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J161" s="3">
+        <v>100</v>
+      </c>
+      <c r="K161" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L161" s="5">
+        <v>0.91071428571428503</v>
+      </c>
+      <c r="M161" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="N161" s="5">
+        <v>0.871428571428571</v>
+      </c>
+      <c r="O161" s="5">
+        <v>0.83571428571428497</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A162" s="3">
+        <v>3</v>
+      </c>
+      <c r="B162" s="3">
+        <v>2</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D162" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F162" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G162" s="3">
+        <v>2</v>
+      </c>
+      <c r="H162" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I162" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J162" s="3">
+        <v>100</v>
+      </c>
+      <c r="K162" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L162" s="5">
+        <v>0.94642857142857095</v>
+      </c>
+      <c r="M162" s="5">
+        <v>1</v>
+      </c>
+      <c r="N162" s="5">
+        <v>0.92321428571428499</v>
+      </c>
+      <c r="O162" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A163" s="3">
+        <v>3</v>
+      </c>
+      <c r="B163" s="3">
+        <v>2</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D163" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F163" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G163" s="3">
+        <v>3</v>
+      </c>
+      <c r="H163" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I163" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J163" s="3">
+        <v>100</v>
+      </c>
+      <c r="K163" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L163" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M163" s="5">
+        <v>1</v>
+      </c>
+      <c r="N163" s="5">
+        <v>0.96071428571428497</v>
+      </c>
+      <c r="O163" s="5">
+        <v>0.90714285714285703</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A164" s="3">
+        <v>4</v>
+      </c>
+      <c r="B164" s="3">
+        <v>0</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D164" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G164" s="3">
+        <v>1</v>
+      </c>
+      <c r="H164" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I164" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J164" s="3">
+        <v>100</v>
+      </c>
+      <c r="K164" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L164" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="M164" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="N164" s="5">
+        <v>0.88749999999999996</v>
+      </c>
+      <c r="O164" s="5">
+        <v>0.84285714285714197</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A165" s="3">
+        <v>4</v>
+      </c>
+      <c r="B165" s="3">
+        <v>0</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D165" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G165" s="3">
+        <v>2</v>
+      </c>
+      <c r="H165" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I165" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J165" s="3">
+        <v>100</v>
+      </c>
+      <c r="K165" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L165" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M165" s="5">
+        <v>1</v>
+      </c>
+      <c r="N165" s="5">
+        <v>0.95178571428571401</v>
+      </c>
+      <c r="O165" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A166" s="3">
+        <v>4</v>
+      </c>
+      <c r="B166" s="3">
+        <v>0</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D166" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G166" s="3">
+        <v>3</v>
+      </c>
+      <c r="H166" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I166" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J166" s="3">
+        <v>100</v>
+      </c>
+      <c r="K166" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L166" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M166" s="5">
+        <v>1</v>
+      </c>
+      <c r="N166" s="5">
+        <v>0.97857142857142798</v>
+      </c>
+      <c r="O166" s="5">
+        <v>0.97142857142857097</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A167" s="3">
+        <v>4</v>
+      </c>
+      <c r="B167" s="3">
+        <v>1</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D167" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G167" s="3">
+        <v>1</v>
+      </c>
+      <c r="H167" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I167" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J167" s="3">
+        <v>100</v>
+      </c>
+      <c r="K167" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L167" s="5">
+        <v>0.89285714285714202</v>
+      </c>
+      <c r="M167" s="5">
+        <v>0.85714285714285698</v>
+      </c>
+      <c r="N167" s="5">
+        <v>0.86607142857142805</v>
+      </c>
+      <c r="O167" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A168" s="3">
+        <v>4</v>
+      </c>
+      <c r="B168" s="3">
+        <v>1</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D168" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G168" s="3">
+        <v>2</v>
+      </c>
+      <c r="H168" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I168" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J168" s="3">
+        <v>100</v>
+      </c>
+      <c r="K168" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L168" s="5">
+        <v>1</v>
+      </c>
+      <c r="M168" s="5">
+        <v>1</v>
+      </c>
+      <c r="N168" s="5">
+        <v>0.941071428571428</v>
+      </c>
+      <c r="O168" s="5">
+        <v>0.92142857142857104</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A169" s="3">
+        <v>4</v>
+      </c>
+      <c r="B169" s="3">
+        <v>1</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D169" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G169" s="3">
+        <v>3</v>
+      </c>
+      <c r="H169" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I169" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J169" s="3">
+        <v>100</v>
+      </c>
+      <c r="K169" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L169" s="5">
+        <v>1</v>
+      </c>
+      <c r="M169" s="5">
+        <v>1</v>
+      </c>
+      <c r="N169" s="5">
+        <v>0.95892857142857102</v>
+      </c>
+      <c r="O169" s="5">
+        <v>0.91428571428571404</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A170" s="3">
+        <v>4</v>
+      </c>
+      <c r="B170" s="3">
+        <v>2</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D170" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G170" s="3">
+        <v>1</v>
+      </c>
+      <c r="H170" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I170" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J170" s="3">
+        <v>100</v>
+      </c>
+      <c r="K170" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L170" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="M170" s="5">
+        <v>0.85714285714285698</v>
+      </c>
+      <c r="N170" s="5">
+        <v>0.84821428571428503</v>
+      </c>
+      <c r="O170" s="5">
+        <v>0.75714285714285701</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A171" s="3">
+        <v>4</v>
+      </c>
+      <c r="B171" s="3">
+        <v>2</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D171" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F171" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G171" s="3">
+        <v>2</v>
+      </c>
+      <c r="H171" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I171" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J171" s="3">
+        <v>100</v>
+      </c>
+      <c r="K171" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L171" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="M171" s="5">
+        <v>1</v>
+      </c>
+      <c r="N171" s="5">
+        <v>0.91428571428571404</v>
+      </c>
+      <c r="O171" s="5">
+        <v>0.99285714285714199</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A172" s="3">
+        <v>4</v>
+      </c>
+      <c r="B172" s="3">
+        <v>2</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D172" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E172" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G172" s="3">
+        <v>3</v>
+      </c>
+      <c r="H172" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I172" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J172" s="3">
+        <v>100</v>
+      </c>
+      <c r="K172" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L172" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M172" s="5">
+        <v>1</v>
+      </c>
+      <c r="N172" s="5">
+        <v>0.94464285714285701</v>
+      </c>
+      <c r="O172" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A173" s="3">
+        <v>5</v>
+      </c>
+      <c r="B173" s="3">
+        <v>0</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D173" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E173" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F173" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G173" s="3">
+        <v>1</v>
+      </c>
+      <c r="H173" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I173" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J173" s="3">
+        <v>100</v>
+      </c>
+      <c r="K173" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L173" s="5">
+        <v>0.94642857142857095</v>
+      </c>
+      <c r="M173" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="N173" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="O173" s="5">
+        <v>0.89285714285714202</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A174" s="3">
+        <v>5</v>
+      </c>
+      <c r="B174" s="3">
+        <v>0</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D174" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F174" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G174" s="3">
+        <v>2</v>
+      </c>
+      <c r="H174" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I174" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J174" s="3">
+        <v>100</v>
+      </c>
+      <c r="K174" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L174" s="5">
+        <v>1</v>
+      </c>
+      <c r="M174" s="5">
+        <v>1</v>
+      </c>
+      <c r="N174" s="5">
+        <v>0.97142857142857097</v>
+      </c>
+      <c r="O174" s="5">
+        <v>0.97142857142857097</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A175" s="3">
+        <v>5</v>
+      </c>
+      <c r="B175" s="3">
+        <v>0</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D175" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F175" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G175" s="3">
+        <v>3</v>
+      </c>
+      <c r="H175" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I175" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J175" s="3">
+        <v>100</v>
+      </c>
+      <c r="K175" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L175" s="5">
+        <v>1</v>
+      </c>
+      <c r="M175" s="5">
+        <v>1</v>
+      </c>
+      <c r="N175" s="5">
+        <v>0.98392857142857104</v>
+      </c>
+      <c r="O175" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A176" s="3">
+        <v>5</v>
+      </c>
+      <c r="B176" s="3">
+        <v>1</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D176" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F176" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G176" s="3">
+        <v>1</v>
+      </c>
+      <c r="H176" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I176" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J176" s="3">
+        <v>100</v>
+      </c>
+      <c r="K176" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L176" s="5">
+        <v>0.94642857142857095</v>
+      </c>
+      <c r="M176" s="5">
+        <v>1</v>
+      </c>
+      <c r="N176" s="5">
+        <v>0.91785714285714204</v>
+      </c>
+      <c r="O176" s="5">
+        <v>0.871428571428571</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A177" s="3">
+        <v>5</v>
+      </c>
+      <c r="B177" s="3">
+        <v>1</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D177" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F177" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G177" s="3">
+        <v>2</v>
+      </c>
+      <c r="H177" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I177" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J177" s="3">
+        <v>100</v>
+      </c>
+      <c r="K177" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L177" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="M177" s="5">
+        <v>1</v>
+      </c>
+      <c r="N177" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="O177" s="5">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A178" s="3">
+        <v>5</v>
+      </c>
+      <c r="B178" s="3">
+        <v>1</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D178" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F178" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G178" s="3">
+        <v>3</v>
+      </c>
+      <c r="H178" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I178" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J178" s="3">
+        <v>100</v>
+      </c>
+      <c r="K178" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L178" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M178" s="5">
+        <v>1</v>
+      </c>
+      <c r="N178" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="O178" s="5">
+        <v>0.97857142857142798</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A179" s="3">
+        <v>5</v>
+      </c>
+      <c r="B179" s="3">
+        <v>2</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D179" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F179" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G179" s="3">
+        <v>1</v>
+      </c>
+      <c r="H179" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I179" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J179" s="3">
+        <v>100</v>
+      </c>
+      <c r="K179" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L179" s="5">
+        <v>0.94642857142857095</v>
+      </c>
+      <c r="M179" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+      <c r="N179" s="5">
+        <v>0.85357142857142798</v>
+      </c>
+      <c r="O179" s="5">
+        <v>0.77142857142857102</v>
+      </c>
+    </row>
+    <row r="180" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A180" s="3">
+        <v>5</v>
+      </c>
+      <c r="B180" s="3">
+        <v>2</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D180" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F180" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G180" s="3">
+        <v>2</v>
+      </c>
+      <c r="H180" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I180" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J180" s="3">
+        <v>100</v>
+      </c>
+      <c r="K180" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L180" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="M180" s="5">
+        <v>1</v>
+      </c>
+      <c r="N180" s="5">
+        <v>0.93928571428571395</v>
+      </c>
+      <c r="O180" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A181" s="3">
+        <v>5</v>
+      </c>
+      <c r="B181" s="3">
+        <v>2</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D181" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F181" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G181" s="3">
+        <v>3</v>
+      </c>
+      <c r="H181" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I181" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J181" s="3">
+        <v>100</v>
+      </c>
+      <c r="K181" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L181" s="5">
+        <v>0.98214285714285698</v>
+      </c>
+      <c r="M181" s="5">
+        <v>1</v>
+      </c>
+      <c r="N181" s="5">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="O181" s="5">
+        <v>0.92857142857142805</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>